<commit_message>
add excel for case31 and case32
</commit_message>
<xml_diff>
--- a/Problem/Case_2_result.xlsx
+++ b/Problem/Case_2_result.xlsx
@@ -368,7 +368,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6226,7 +6226,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -11118,7 +11118,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>